<commit_message>
Finished working on GRU model
</commit_message>
<xml_diff>
--- a/results/LIN/linear_models.xlsx
+++ b/results/LIN/linear_models.xlsx
@@ -470,19 +470,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.004769122965975618</v>
+        <v>0.004963351638465073</v>
       </c>
       <c r="C2" t="n">
-        <v>0.004837348405401622</v>
+        <v>0.004834212512253471</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9817094180775661</v>
+        <v>0.9906736939747048</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9817042844946174</v>
+        <v>0.9634655839616465</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8298432984162167</v>
+        <v>0.2594227710945805</v>
       </c>
     </row>
     <row r="3">
@@ -490,19 +490,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.003695070703817236</v>
+        <v>0.003770732141401472</v>
       </c>
       <c r="C3" t="n">
-        <v>0.003754690403780813</v>
+        <v>0.00361547136886158</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9858287049803403</v>
+        <v>0.9929146693285493</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9857990650413668</v>
+        <v>0.9726752168337587</v>
       </c>
       <c r="F3" t="n">
-        <v>0.951116065724943</v>
+        <v>0.4372503071926935</v>
       </c>
     </row>
     <row r="4">
@@ -510,19 +510,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.003386840317807086</v>
+        <v>0.003429803662143611</v>
       </c>
       <c r="C4" t="n">
-        <v>0.003432796726155553</v>
+        <v>0.003264441653402447</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9870109779309727</v>
+        <v>0.9935552878583357</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9870165428189214</v>
+        <v>0.9753268970896201</v>
       </c>
       <c r="F4" t="n">
-        <v>1.028017927903523</v>
+        <v>0.5000027187813955</v>
       </c>
     </row>
     <row r="5">
@@ -530,19 +530,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.00327315014932248</v>
+        <v>0.003292163988191401</v>
       </c>
       <c r="C5" t="n">
-        <v>0.003322526532289555</v>
+        <v>0.003103780506519008</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9874470913775609</v>
+        <v>0.9938139233952664</v>
       </c>
       <c r="E5" t="n">
-        <v>0.987433505121374</v>
+        <v>0.9765406859767927</v>
       </c>
       <c r="F5" t="n">
-        <v>1.060811013861573</v>
+        <v>0.5289152812660634</v>
       </c>
     </row>
     <row r="6">
@@ -550,19 +550,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.00321467702370008</v>
+        <v>0.003235555690129871</v>
       </c>
       <c r="C6" t="n">
-        <v>0.003259960989261046</v>
+        <v>0.003018017049313306</v>
       </c>
       <c r="D6" t="n">
-        <v>0.987671519492764</v>
+        <v>0.9939203066067568</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9876701241456329</v>
+        <v>0.977188336127628</v>
       </c>
       <c r="F6" t="n">
-        <v>1.074759087522958</v>
+        <v>0.5464952269244026</v>
       </c>
     </row>
     <row r="7">
@@ -570,19 +570,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.003184661718274264</v>
+        <v>0.003215636986979346</v>
       </c>
       <c r="C7" t="n">
-        <v>0.003238196728804748</v>
+        <v>0.002978544582061501</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9877867043829439</v>
+        <v>0.9939577344190823</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9877522261865517</v>
+        <v>0.9774861471260623</v>
       </c>
       <c r="F7" t="n">
-        <v>1.081653301003036</v>
+        <v>0.5566465993413788</v>
       </c>
     </row>
     <row r="8">
@@ -590,19 +590,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.003169567311476295</v>
+        <v>0.003208329051028374</v>
       </c>
       <c r="C8" t="n">
-        <v>0.003226463537764576</v>
+        <v>0.002958976679893763</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9878447223659332</v>
+        <v>0.9939714694491053</v>
       </c>
       <c r="E8" t="n">
-        <v>0.987796413504525</v>
+        <v>0.9776332370965403</v>
       </c>
       <c r="F8" t="n">
-        <v>1.08402882354076</v>
+        <v>0.5616437937463485</v>
       </c>
     </row>
     <row r="9">
@@ -610,19 +610,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.003164834412751226</v>
+        <v>0.003204016641743583</v>
       </c>
       <c r="C9" t="n">
-        <v>0.003221627470404254</v>
+        <v>0.0029553215929497</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9878630527204592</v>
+        <v>0.9939795698876578</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9878146989455669</v>
+        <v>0.9776607381133388</v>
       </c>
       <c r="F9" t="n">
-        <v>1.086247391140893</v>
+        <v>0.5760438850718214</v>
       </c>
     </row>
     <row r="10">
@@ -630,19 +630,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.003162531201410408</v>
+        <v>0.00319974991137509</v>
       </c>
       <c r="C10" t="n">
-        <v>0.003216310497246766</v>
+        <v>0.002959257475508847</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9878719776237154</v>
+        <v>0.9939875851829847</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9878350479592899</v>
+        <v>0.9776308360184502</v>
       </c>
       <c r="F10" t="n">
-        <v>1.086441833935067</v>
+        <v>0.5876316320306215</v>
       </c>
     </row>
     <row r="11">
@@ -650,19 +650,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.003161311503643271</v>
+        <v>0.003195457044718022</v>
       </c>
       <c r="C11" t="n">
-        <v>0.003214497651532622</v>
+        <v>0.002964026638212515</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9878767374768066</v>
+        <v>0.9939956362676579</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9878419362653942</v>
+        <v>0.9775943548661169</v>
       </c>
       <c r="F11" t="n">
-        <v>1.0862688935773</v>
+        <v>0.5979775984913919</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GRU MPC working but with low performance (still :( )
</commit_message>
<xml_diff>
--- a/results/LIN/linear_models.xlsx
+++ b/results/LIN/linear_models.xlsx
@@ -470,19 +470,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.004963351638465073</v>
+        <v>0.004958007358721677</v>
       </c>
       <c r="C2" t="n">
-        <v>0.004834212512253471</v>
+        <v>0.004861074973228985</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9906736939747048</v>
+        <v>0.9903417954640102</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9634655839616465</v>
+        <v>0.957446478056866</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2594227710945805</v>
+        <v>0.03327798622130068</v>
       </c>
     </row>
     <row r="3">
@@ -490,19 +490,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.003770732141401472</v>
+        <v>0.003739810559255043</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00361547136886158</v>
+        <v>0.003653747881690812</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9929146693285493</v>
+        <v>0.9927148204291156</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9726752168337587</v>
+        <v>0.9680131162517521</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4372503071926935</v>
+        <v>0.01326005264751901</v>
       </c>
     </row>
     <row r="4">
@@ -510,19 +510,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.003429803662143611</v>
+        <v>0.003405827010953281</v>
       </c>
       <c r="C4" t="n">
-        <v>0.003264441653402447</v>
+        <v>0.003314319779483316</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9935552878583357</v>
+        <v>0.9933654155001719</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9753268970896201</v>
+        <v>0.9709827628938295</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5000027187813955</v>
+        <v>0.01429345732811882</v>
       </c>
     </row>
     <row r="5">
@@ -530,19 +530,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.003292163988191401</v>
+        <v>0.003257129333634557</v>
       </c>
       <c r="C5" t="n">
-        <v>0.003103780506519008</v>
+        <v>0.003140833072028297</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9938139233952664</v>
+        <v>0.9936550565119737</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9765406859767927</v>
+        <v>0.9725002170295135</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5289152812660634</v>
+        <v>0.01386102876658908</v>
       </c>
     </row>
     <row r="6">
@@ -550,19 +550,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.003235555690129871</v>
+        <v>0.003192107076096309</v>
       </c>
       <c r="C6" t="n">
-        <v>0.003018017049313306</v>
+        <v>0.003040422155846522</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9939203066067568</v>
+        <v>0.9937817207758056</v>
       </c>
       <c r="E6" t="n">
-        <v>0.977188336127628</v>
+        <v>0.9733784427813837</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5464952269244026</v>
+        <v>0.01384516524969282</v>
       </c>
     </row>
     <row r="7">
@@ -570,19 +570,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.003215636986979346</v>
+        <v>0.003163942208685931</v>
       </c>
       <c r="C7" t="n">
-        <v>0.002978544582061501</v>
+        <v>0.00299182578862744</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9939577344190823</v>
+        <v>0.9938365950173765</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9774861471260623</v>
+        <v>0.9738030155393282</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5566465993413788</v>
+        <v>0.01417268802553237</v>
       </c>
     </row>
     <row r="8">
@@ -590,19 +590,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.003208329051028374</v>
+        <v>0.0031532551802971</v>
       </c>
       <c r="C8" t="n">
-        <v>0.002958976679893763</v>
+        <v>0.002965733558919699</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9939714694491053</v>
+        <v>0.993857414701213</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9776332370965403</v>
+        <v>0.9740306548814219</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5616437937463485</v>
+        <v>0.01401041383150893</v>
       </c>
     </row>
     <row r="9">
@@ -610,19 +610,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.003204016641743583</v>
+        <v>0.003149388712457963</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0029553215929497</v>
+        <v>0.00295561973124334</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9939795698876578</v>
+        <v>0.9938649480363753</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9776607381133388</v>
+        <v>0.9741189114538299</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5760438850718214</v>
+        <v>0.01384946254290247</v>
       </c>
     </row>
     <row r="10">
@@ -630,19 +630,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.00319974991137509</v>
+        <v>0.003147323221355497</v>
       </c>
       <c r="C10" t="n">
-        <v>0.002959257475508847</v>
+        <v>0.002954008572207624</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9939875851829847</v>
+        <v>0.9938689686819906</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9776308360184502</v>
+        <v>0.9741324929757319</v>
       </c>
       <c r="F10" t="n">
-        <v>0.5876316320306215</v>
+        <v>0.01373682671195912</v>
       </c>
     </row>
     <row r="11">
@@ -650,19 +650,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.003195457044718022</v>
+        <v>0.003145267823882309</v>
       </c>
       <c r="C11" t="n">
-        <v>0.002964026638212515</v>
+        <v>0.002955946713526951</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9939956362676579</v>
+        <v>0.9938729814491797</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9775943548661169</v>
+        <v>0.9741145774834474</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5979775984913919</v>
+        <v>0.01378774163131053</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for more figures
</commit_message>
<xml_diff>
--- a/results/LIN/linear_models.xlsx
+++ b/results/LIN/linear_models.xlsx
@@ -1,37 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Linear" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Linear" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>ks</t>
+  </si>
+  <si>
+    <t>MSE_tr</t>
+  </si>
+  <si>
+    <t>MSE_te</t>
+  </si>
+  <si>
+    <t>R2 train</t>
+  </si>
+  <si>
+    <t>R2 test</t>
+  </si>
+  <si>
+    <t>MSE_offline</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +72,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,252 +388,234 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ks</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>MSE_tr</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>MSE_te</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>R2 train</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>R2 test</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>MSE_offline</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>0.004958007358721677</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.004861074973228985</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="C2">
+        <v>0.00486107497322899</v>
+      </c>
+      <c r="D2">
         <v>0.9903417954640102</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>0.957446478056866</v>
       </c>
-      <c r="F2" t="n">
-        <v>0.03327798622130068</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+      <c r="F2">
+        <v>0.03327798622128499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
-        <v>0.003739810559255043</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.003653747881690812</v>
-      </c>
-      <c r="D3" t="n">
+      <c r="B3">
+        <v>0.003739810559255044</v>
+      </c>
+      <c r="C3">
+        <v>0.003653747881690813</v>
+      </c>
+      <c r="D3">
         <v>0.9927148204291156</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>0.9680131162517521</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.01326005264751901</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
+      <c r="F3">
+        <v>0.01326005264751999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>0.003405827010953281</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.003314319779483316</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4">
+        <v>0.00331431977948331</v>
+      </c>
+      <c r="D4">
         <v>0.9933654155001719</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.9709827628938295</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.01429345732811882</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
+      <c r="E4">
+        <v>0.9709827628938296</v>
+      </c>
+      <c r="F4">
+        <v>0.01429345732811591</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>0.003257129333634557</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.003140833072028297</v>
-      </c>
-      <c r="D5" t="n">
+      <c r="C5">
+        <v>0.003140833072028293</v>
+      </c>
+      <c r="D5">
         <v>0.9936550565119737</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>0.9725002170295135</v>
       </c>
-      <c r="F5" t="n">
-        <v>0.01386102876658908</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
+      <c r="F5">
+        <v>0.01386102876658648</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>0.003192107076096309</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.003040422155846522</v>
-      </c>
-      <c r="D6" t="n">
+      <c r="C6">
+        <v>0.003040422155846519</v>
+      </c>
+      <c r="D6">
         <v>0.9937817207758056</v>
       </c>
-      <c r="E6" t="n">
-        <v>0.9733784427813837</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.01384516524969282</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
+      <c r="E6">
+        <v>0.9733784427813839</v>
+      </c>
+      <c r="F6">
+        <v>0.01384516524969166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>0.003163942208685931</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.00299182578862744</v>
-      </c>
-      <c r="D7" t="n">
+      <c r="C7">
+        <v>0.002991825788627438</v>
+      </c>
+      <c r="D7">
         <v>0.9938365950173765</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>0.9738030155393282</v>
       </c>
-      <c r="F7" t="n">
-        <v>0.01417268802553237</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
+      <c r="F7">
+        <v>0.01417268802553101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>0.0031532551802971</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.002965733558919699</v>
-      </c>
-      <c r="D8" t="n">
+      <c r="C8">
+        <v>0.002965733558919704</v>
+      </c>
+      <c r="D8">
         <v>0.993857414701213</v>
       </c>
-      <c r="E8" t="n">
-        <v>0.9740306548814219</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.01401041383150893</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
+      <c r="E8">
+        <v>0.9740306548814218</v>
+      </c>
+      <c r="F8">
+        <v>0.01401041383151079</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
-        <v>0.003149388712457963</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.00295561973124334</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="B9">
+        <v>0.003149388712457964</v>
+      </c>
+      <c r="C9">
+        <v>0.002955619731243339</v>
+      </c>
+      <c r="D9">
         <v>0.9938649480363753</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>0.9741189114538299</v>
       </c>
-      <c r="F9" t="n">
-        <v>0.01384946254290247</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
+      <c r="F9">
+        <v>0.01384946254290059</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
-        <v>0.003147323221355497</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.002954008572207624</v>
-      </c>
-      <c r="D10" t="n">
+      <c r="B10">
+        <v>0.003147323221355499</v>
+      </c>
+      <c r="C10">
+        <v>0.002954008572207621</v>
+      </c>
+      <c r="D10">
         <v>0.9938689686819906</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>0.9741324929757319</v>
       </c>
-      <c r="F10" t="n">
-        <v>0.01373682671195912</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
+      <c r="F10">
+        <v>0.01373682671195651</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="n">
-        <v>0.003145267823882309</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.002955946713526951</v>
-      </c>
-      <c r="D11" t="n">
+      <c r="B11">
+        <v>0.00314526782388231</v>
+      </c>
+      <c r="C11">
+        <v>0.002955946713526945</v>
+      </c>
+      <c r="D11">
         <v>0.9938729814491797</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>0.9741145774834474</v>
       </c>
-      <c r="F11" t="n">
-        <v>0.01378774163131053</v>
+      <c r="F11">
+        <v>0.01378774163130827</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed the get error function and bugfix -> models working better but still slow
</commit_message>
<xml_diff>
--- a/results/LIN/linear_models.xlsx
+++ b/results/LIN/linear_models.xlsx
@@ -470,19 +470,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.005016436983894019</v>
+        <v>0.005008895563459881</v>
       </c>
       <c r="C2" t="n">
-        <v>0.004906187965681635</v>
+        <v>0.004865247036065751</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9907369743618991</v>
+        <v>0.9923521113034691</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9704915805119965</v>
+        <v>0.9699837656733843</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1254200005790063</v>
+        <v>0.02507164465589896</v>
       </c>
     </row>
     <row r="3">
@@ -490,19 +490,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.003805403845907612</v>
+        <v>0.00380692192223831</v>
       </c>
       <c r="C3" t="n">
-        <v>0.003683640409632276</v>
+        <v>0.003683159766929739</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9929731964342249</v>
+        <v>0.9941873923600733</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9778440043856748</v>
+        <v>0.9772766546732718</v>
       </c>
       <c r="F3" t="n">
-        <v>0.08233186721496623</v>
+        <v>0.06480254347562245</v>
       </c>
     </row>
     <row r="4">
@@ -510,19 +510,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.00346985875074054</v>
+        <v>0.003443900295586771</v>
       </c>
       <c r="C4" t="n">
-        <v>0.003341700074978395</v>
+        <v>0.003317591456365003</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9935927870867062</v>
+        <v>0.9947417028378188</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9799002343392899</v>
+        <v>0.9795318532006546</v>
       </c>
       <c r="F4" t="n">
-        <v>0.07673030349605499</v>
+        <v>0.096012353089812</v>
       </c>
     </row>
     <row r="5">
@@ -530,19 +530,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.003338655119090103</v>
+        <v>0.003279752094924345</v>
       </c>
       <c r="C5" t="n">
-        <v>0.003166897244336493</v>
+        <v>0.00317266758868667</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9938350570600186</v>
+        <v>0.99499236075113</v>
       </c>
       <c r="E5" t="n">
-        <v>0.980951014344337</v>
+        <v>0.9804260252982087</v>
       </c>
       <c r="F5" t="n">
-        <v>0.07922783308160548</v>
+        <v>0.1170764944447394</v>
       </c>
     </row>
     <row r="6">
@@ -550,19 +550,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.003285796486398086</v>
+        <v>0.003203882065447422</v>
       </c>
       <c r="C6" t="n">
-        <v>0.003093581071971527</v>
+        <v>0.003090791739249922</v>
       </c>
       <c r="D6" t="n">
-        <v>0.993932662087502</v>
+        <v>0.9951082300976939</v>
       </c>
       <c r="E6" t="n">
-        <v>0.981391382274907</v>
+        <v>0.9809310720990054</v>
       </c>
       <c r="F6" t="n">
-        <v>0.07631142277773895</v>
+        <v>0.1243068192719438</v>
       </c>
     </row>
     <row r="7">
@@ -570,19 +570,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.003263457902392758</v>
+        <v>0.003164966658204907</v>
       </c>
       <c r="C7" t="n">
-        <v>0.003053079469580526</v>
+        <v>0.003043448822865191</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9939739007237698</v>
+        <v>0.9951676752613348</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9816342531307641</v>
+        <v>0.9812230747765913</v>
       </c>
       <c r="F7" t="n">
-        <v>0.07489024784754869</v>
+        <v>0.119294387541022</v>
       </c>
     </row>
     <row r="8">
@@ -590,19 +590,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.003257333194046959</v>
+        <v>0.003146941067278173</v>
       </c>
       <c r="C8" t="n">
-        <v>0.00303967860264211</v>
+        <v>0.003016007962439752</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9939852110812555</v>
+        <v>0.9951952251388529</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9817144320093926</v>
+        <v>0.9813923596696512</v>
       </c>
       <c r="F8" t="n">
-        <v>0.07483353304407209</v>
+        <v>0.1207705991839658</v>
       </c>
     </row>
     <row r="9">
@@ -610,19 +610,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.003253915391433458</v>
+        <v>0.003139860118486467</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00303541185407594</v>
+        <v>0.003000730289103017</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9939915382007439</v>
+        <v>0.9952060644861318</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9817398612976234</v>
+        <v>0.9814861915264435</v>
       </c>
       <c r="F9" t="n">
-        <v>0.07453744825186427</v>
+        <v>0.1197290582431418</v>
       </c>
     </row>
     <row r="10">
@@ -630,19 +630,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.003251442885058119</v>
+        <v>0.003136161325357725</v>
       </c>
       <c r="C10" t="n">
-        <v>0.003037686950549426</v>
+        <v>0.002997739211620087</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9939961193280104</v>
+        <v>0.9952117393333206</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9817257165718178</v>
+        <v>0.9815047699399906</v>
       </c>
       <c r="F10" t="n">
-        <v>0.07617729292134418</v>
+        <v>0.1358383762365296</v>
       </c>
     </row>
     <row r="11">
@@ -650,19 +650,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.003247551799173775</v>
+        <v>0.003133808574706114</v>
       </c>
       <c r="C11" t="n">
-        <v>0.003039897321017599</v>
+        <v>0.002997170306043766</v>
       </c>
       <c r="D11" t="n">
-        <v>0.994003314286565</v>
+        <v>0.9952153586996393</v>
       </c>
       <c r="E11" t="n">
-        <v>0.981712243279838</v>
+        <v>0.9815080928066962</v>
       </c>
       <c r="F11" t="n">
-        <v>0.07643316992878096</v>
+        <v>0.1325553389826539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>